<commit_message>
adding all modules to excel
</commit_message>
<xml_diff>
--- a/Online-Portals/PreBuilding/TestCases.xlsx
+++ b/Online-Portals/PreBuilding/TestCases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Pass</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>CSR_Regression</t>
+  </si>
+  <si>
+    <t>Enrollment Flow</t>
+  </si>
+  <si>
+    <t>test.java.TestUPAEnrollment</t>
+  </si>
+  <si>
+    <t>My Profile</t>
+  </si>
+  <si>
+    <t>test.java.TestUPAMyProfileTab</t>
   </si>
 </sst>
 </file>
@@ -437,10 +449,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,12 +497,34 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing according to new code going in release
</commit_message>
<xml_diff>
--- a/Online-Portals/PreBuilding/TestCases.xlsx
+++ b/Online-Portals/PreBuilding/TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20496" windowHeight="7560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BLOOM" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,7 +522,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
test cases in xml
</commit_message>
<xml_diff>
--- a/Online-Portals/PreBuilding/TestCases.xlsx
+++ b/Online-Portals/PreBuilding/TestCases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Pass</t>
   </si>
@@ -80,7 +80,25 @@
     <t>View Payments</t>
   </si>
   <si>
-    <t>test.java.TestViewPayments</t>
+    <t>Provider View Payments</t>
+  </si>
+  <si>
+    <t>BS View Payments</t>
+  </si>
+  <si>
+    <t>Payer View Payments</t>
+  </si>
+  <si>
+    <t>test.java.TestProviderViewPayments</t>
+  </si>
+  <si>
+    <t>test.java.TestBSViewPayments</t>
+  </si>
+  <si>
+    <t>test.java.TestPayerViewPayments</t>
+  </si>
+  <si>
+    <t>TestCSRViewPayments</t>
   </si>
 </sst>
 </file>
@@ -404,7 +422,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -455,10 +473,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,10 +535,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -528,21 +546,54 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing test creste enrollment module into test case excel file
</commit_message>
<xml_diff>
--- a/Online-Portals/PreBuilding/TestCases.xlsx
+++ b/Online-Portals/PreBuilding/TestCases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Pass</t>
   </si>
@@ -98,7 +98,13 @@
     <t>test.java.TestPayerViewPayments</t>
   </si>
   <si>
-    <t>TestCSRViewPayments</t>
+    <t>test.java.TestCSRViewPayments</t>
+  </si>
+  <si>
+    <t>Create Enrollment</t>
+  </si>
+  <si>
+    <t>test.java.TestCreateEnrollment</t>
   </si>
 </sst>
 </file>
@@ -422,7 +428,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -473,10 +479,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,6 +600,17 @@
       </c>
       <c r="C10" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge pull request #18 from EPS-Automation/US1023501_TINStatusPages"
This reverts commit cc821e9096d4bc0a38ca3f221b2a6b75a90fc487, reversing
changes made to 6af6a1581180e61980d9d9328001225615a0d0a6.
</commit_message>
<xml_diff>
--- a/Online-Portals/PreBuilding/TestCases.xlsx
+++ b/Online-Portals/PreBuilding/TestCases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Pass</t>
   </si>
@@ -98,7 +98,13 @@
     <t>test.java.TestPayerViewPayments</t>
   </si>
   <si>
-    <t>TestCSRViewPayments</t>
+    <t>test.java.TestCSRViewPayments</t>
+  </si>
+  <si>
+    <t>Create Enrollment</t>
+  </si>
+  <si>
+    <t>test.java.TestCreateEnrollment</t>
   </si>
 </sst>
 </file>
@@ -422,7 +428,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -473,10 +479,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,6 +600,17 @@
       </c>
       <c r="C10" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extent reports updated to show categories
</commit_message>
<xml_diff>
--- a/Online-Portals/PreBuilding/TestCases.xlsx
+++ b/Online-Portals/PreBuilding/TestCases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Pass</t>
   </si>
@@ -99,12 +99,6 @@
   </si>
   <si>
     <t>TestCSRViewPayments</t>
-  </si>
-  <si>
-    <t>Create Enrollment</t>
-  </si>
-  <si>
-    <t>test.java.TestCreateEnrollment</t>
   </si>
 </sst>
 </file>
@@ -428,7 +422,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -479,10 +473,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,42 +568,31 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Amit's Create enrollment fixes and updating data file
Amit's Create enrollment fixes and updating data file
</commit_message>
<xml_diff>
--- a/Online-Portals/PreBuilding/TestCases.xlsx
+++ b/Online-Portals/PreBuilding/TestCases.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>Pass</t>
   </si>
@@ -65,12 +65,6 @@
     <t>CSR_Regression</t>
   </si>
   <si>
-    <t>Enrollment Flow</t>
-  </si>
-  <si>
-    <t>test.java.TestUPAEnrollment</t>
-  </si>
-  <si>
     <t>My Profile</t>
   </si>
   <si>
@@ -98,13 +92,37 @@
     <t>test.java.TestPayerViewPayments</t>
   </si>
   <si>
-    <t>TestCSRViewPayments</t>
-  </si>
-  <si>
     <t>Create Enrollment</t>
   </si>
   <si>
     <t>test.java.TestCreateEnrollment</t>
+  </si>
+  <si>
+    <t>Provider Search Remittance</t>
+  </si>
+  <si>
+    <t>test.java.TestProviderSearchRemittance</t>
+  </si>
+  <si>
+    <t>BS Search Remittance</t>
+  </si>
+  <si>
+    <t>test.java.TestBSSearchRemittance</t>
+  </si>
+  <si>
+    <t>SubPayer Search Remittance</t>
+  </si>
+  <si>
+    <t>test.java.TestSubPayerSearchRemittance</t>
+  </si>
+  <si>
+    <t>test.java.TestCSRViewPayments</t>
+  </si>
+  <si>
+    <t>test.java.TestCSRSearchRemittance</t>
+  </si>
+  <si>
+    <t>Search Remittance</t>
   </si>
 </sst>
 </file>
@@ -428,7 +446,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -479,10 +497,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,10 +548,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -541,10 +559,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -552,10 +570,10 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -563,7 +581,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -574,10 +592,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -585,32 +603,65 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>